<commit_message>
Oikean puhelinnumeron nouto YTJ-rekisteristä
</commit_message>
<xml_diff>
--- a/Data/valitut_ostolaskut.xlsx
+++ b/Data/valitut_ostolaskut.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarre\Documents\UiPath\DigiLii_harjoitusty-\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94E682E-9019-4F13-ACF1-EDFAB04D6500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DE693B-9C7B-4CFF-BD77-BF0B50C6BEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{9DFF3181-8E34-40DF-9F0D-6D3E931B5C12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{7B08B76D-F6BC-4875-ACE9-55202793168A}"/>
   </bookViews>
   <sheets>
     <sheet name="Toimittajarekisteri" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="103">
   <si>
     <t>Kuntanro</t>
   </si>
@@ -100,232 +100,253 @@
     <t>0162193-3</t>
   </si>
   <si>
+    <t>Aineet, tarvikkeet ja tavarat</t>
+  </si>
+  <si>
+    <t>Toimisto- ja koulutarvikkeet</t>
+  </si>
+  <si>
+    <t>Lapset ja nuoret</t>
+  </si>
+  <si>
+    <t>Perusopetus</t>
+  </si>
+  <si>
     <t>Palvelujen ostot</t>
   </si>
   <si>
+    <t>Yhteiset palvelut</t>
+  </si>
+  <si>
+    <t>Konsernin yhteiset</t>
+  </si>
+  <si>
+    <t>ICT-palvelut</t>
+  </si>
+  <si>
+    <t>Kaupunkikehitys</t>
+  </si>
+  <si>
+    <t>Kadut ja ympäristö</t>
+  </si>
+  <si>
+    <t>Rak.ja al.rak.-ja kunn.pitopal</t>
+  </si>
+  <si>
     <t>Tilakeskus</t>
   </si>
   <si>
-    <t>Lapset ja nuoret</t>
-  </si>
-  <si>
-    <t>Perusopetus</t>
-  </si>
-  <si>
-    <t>Aineet, tarvikkeet ja tavarat</t>
-  </si>
-  <si>
-    <t>Toimisto- ja koulutarvikkeet</t>
-  </si>
-  <si>
-    <t>Yhteiset palvelut</t>
-  </si>
-  <si>
-    <t>Konsernin yhteiset</t>
-  </si>
-  <si>
-    <t>Kaupunkikehitys</t>
+    <t>2416249-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUATTROSERVICES KAAKKOISSUOMI     </t>
+  </si>
+  <si>
+    <t>Aineelliset hyödykkeet</t>
+  </si>
+  <si>
+    <t>Keskeneräiset muut rakennukset</t>
+  </si>
+  <si>
+    <t>Investoinnit</t>
+  </si>
+  <si>
+    <t>2246772-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VELIMARK OY     </t>
+  </si>
+  <si>
+    <t>Puhdistusaineet ja -tarvikkeet</t>
+  </si>
+  <si>
+    <t>Muut palvelut</t>
   </si>
   <si>
     <t>Liikuntapalvelut</t>
   </si>
   <si>
-    <t>Kadut ja ympäristö</t>
-  </si>
-  <si>
-    <t>Rak.ja al.rak.-ja kunn.pitopal</t>
+    <t>Ulkoliikuntapaikat</t>
+  </si>
+  <si>
+    <t>2302414-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULOSOTTOLAITOS      </t>
+  </si>
+  <si>
+    <t>Muut kulut</t>
+  </si>
+  <si>
+    <t>Muut toimintakulut</t>
+  </si>
+  <si>
+    <t>1840913-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPR KONTTORIKONE OY    </t>
   </si>
   <si>
     <t>Asiantuntijapalvelut</t>
   </si>
   <si>
-    <t>Ulkoliikuntapaikat</t>
+    <t>1544233-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPEAKERSFORUM FINLAND OY AB   </t>
+  </si>
+  <si>
+    <t>Yrityspalvelut / 2021 Elinvoim</t>
+  </si>
+  <si>
+    <t>3018921-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONSILIA SOLUTIONS AB    </t>
+  </si>
+  <si>
+    <t>0981105-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RAKENNUSPINNOITUS RANTANEN OY    </t>
+  </si>
+  <si>
+    <t>1464614-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELLIBS OY     </t>
+  </si>
+  <si>
+    <t>Kirjallisuus</t>
+  </si>
+  <si>
+    <t>Kulttuuripalvelut</t>
+  </si>
+  <si>
+    <t>Kirjasto</t>
+  </si>
+  <si>
+    <t>2043575-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STARK SUOMI OY    </t>
+  </si>
+  <si>
+    <t>2014838-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BISNODE FINLAND OY    </t>
+  </si>
+  <si>
+    <t>0863729-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOIHDE TRUST OY    </t>
+  </si>
+  <si>
+    <t>Kon. kal. laitt. ja rak.kunn.p</t>
+  </si>
+  <si>
+    <t>0943819-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERIFONE FINLAND OY    </t>
+  </si>
+  <si>
+    <t>Ohjaustoiminta</t>
+  </si>
+  <si>
+    <t>1538517-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ETTEPLAN FINLAND OY    </t>
+  </si>
+  <si>
+    <t>1870837-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LYRECO FINLAND OY    </t>
+  </si>
+  <si>
+    <t>2405922-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PORVOON KIRJAKESKUS OY    </t>
+  </si>
+  <si>
+    <t>0583925-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WULFF SOLUTIONS OY    </t>
+  </si>
+  <si>
+    <t>0252139-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPT GROUP OY    </t>
+  </si>
+  <si>
+    <t>Vaatteisto</t>
+  </si>
+  <si>
+    <t>0162170-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-K OSUUSKAUPPA     </t>
   </si>
   <si>
     <t>Majoitus- ja ravitsemupalvelut</t>
   </si>
   <si>
-    <t>ICT-palvelut</t>
-  </si>
-  <si>
-    <t>2416249-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUATTROSERVICES KAAKKOISSUOMI     </t>
-  </si>
-  <si>
-    <t>Aineelliset hyödykkeet</t>
-  </si>
-  <si>
-    <t>Investoinnit</t>
-  </si>
-  <si>
-    <t>1447914-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCANDIC HOTELS OY    </t>
-  </si>
-  <si>
-    <t>2201468-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAKOSALO SOFTWARE OY    </t>
-  </si>
-  <si>
-    <t>Yrityspalvelut / 2021 Elinvoim</t>
-  </si>
-  <si>
-    <t>2487822-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MH-KESKUS OY     </t>
+    <t>Konsernipalvelut</t>
+  </si>
+  <si>
+    <t>1512332-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INDOOR GROUP OY    </t>
+  </si>
+  <si>
+    <t>Maakunnallinen palvelutoiminta</t>
+  </si>
+  <si>
+    <t>Maahanmuuttopalvelut</t>
+  </si>
+  <si>
+    <t>3096299-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HELSINKI DESIGN PRINTERS OY   </t>
   </si>
   <si>
     <t>Muu materiaali</t>
   </si>
   <si>
-    <t>Kulttuuripalvelut</t>
-  </si>
-  <si>
-    <t>Museo</t>
-  </si>
-  <si>
-    <t>2342152-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JI SPORT A/S    </t>
-  </si>
-  <si>
-    <t>2161840-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KOLME KIVEÄ OY/TANG CAPITAL   </t>
-  </si>
-  <si>
-    <t>Konsernijohto</t>
-  </si>
-  <si>
-    <t>1003521-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VR-YHTYMÄ HENKILÖLIIKENNE     </t>
-  </si>
-  <si>
-    <t>Matkustus- ja kuljetuspalvelut</t>
-  </si>
-  <si>
-    <t>2889642-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYÖKALU JA VARAOSA OY LAPPEEN-  </t>
-  </si>
-  <si>
-    <t>0162170-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-K OSUUSKAUPPA     </t>
-  </si>
-  <si>
-    <t>0107801-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ETRA OY     </t>
-  </si>
-  <si>
-    <t>Varaosat</t>
-  </si>
-  <si>
-    <t>1868810-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PURKUPIHA OY     </t>
-  </si>
-  <si>
-    <t>Maaomaisuuden tuotot</t>
-  </si>
-  <si>
-    <t>2056681-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUSEOPEDAGOGINEN YHDISTYS     </t>
-  </si>
-  <si>
-    <t>Muut kulut</t>
-  </si>
-  <si>
-    <t>Muut toimintakulut</t>
-  </si>
-  <si>
-    <t>2302414-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ULOSOTTOLAITOS      </t>
-  </si>
-  <si>
-    <t>1840913-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LPR KONTTORIKONE OY    </t>
-  </si>
-  <si>
-    <t>1544233-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPEAKERSFORUM FINLAND OY AB   </t>
-  </si>
-  <si>
-    <t>Keskeneräiset muut rakennukset</t>
-  </si>
-  <si>
-    <t>3018921-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONSILIA SOLUTIONS AB    </t>
-  </si>
-  <si>
-    <t>0981105-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAKENNUSPINNOITUS RANTANEN OY    </t>
-  </si>
-  <si>
-    <t>2246772-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VELIMARK OY     </t>
-  </si>
-  <si>
-    <t>Puhdistusaineet ja -tarvikkeet</t>
-  </si>
-  <si>
-    <t>1464614-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ELLIBS OY     </t>
-  </si>
-  <si>
-    <t>Kirjallisuus</t>
-  </si>
-  <si>
-    <t>Kirjasto</t>
-  </si>
-  <si>
-    <t>2043575-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STARK SUOMI OY    </t>
-  </si>
-  <si>
     <t>Nimi</t>
   </si>
   <si>
     <t>Puhelinnumero</t>
   </si>
   <si>
-    <t>050 111 2222</t>
-  </si>
-  <si>
-    <t>040 123 4567</t>
+    <t>010 422 4400</t>
+  </si>
+  <si>
+    <t>02 279 3342</t>
+  </si>
+  <si>
+    <t>(09)272702333</t>
+  </si>
+  <si>
+    <t>029 001 3000</t>
+  </si>
+  <si>
+    <t>+358-9-4774330</t>
+  </si>
+  <si>
+    <t>020 720 5500</t>
+  </si>
+  <si>
+    <t>050 514 2656</t>
   </si>
 </sst>
 </file>
@@ -361,9 +382,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,77 +719,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4338DA-227B-415D-A425-7B7B2292D9C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456916FA-A961-4FE8-B738-6A418C191385}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" style="2" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>93</v>
+        <v>94</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
+        <v>44</v>
+      </c>
+      <c r="C2" s="2">
+        <v>103665150</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
+        <v>48</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>95</v>
+        <v>51</v>
+      </c>
+      <c r="C4" s="2">
+        <v>201552990</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
+        <v>33</v>
+      </c>
+      <c r="C5" s="2">
+        <v>941301239</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>94</v>
+        <v>54</v>
+      </c>
+      <c r="C6" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -777,30 +804,30 @@
       <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>94</v>
+      <c r="C7" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" t="s">
-        <v>94</v>
+        <v>38</v>
+      </c>
+      <c r="C8" s="2">
+        <v>22510231</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" t="s">
-        <v>94</v>
+        <v>58</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -810,96 +837,96 @@
       <c r="B10" t="s">
         <v>63</v>
       </c>
-      <c r="C10" t="s">
-        <v>94</v>
+      <c r="C10" s="2">
+        <v>935413000</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
         <v>65</v>
       </c>
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" t="s">
-        <v>94</v>
+      <c r="C11" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" t="s">
-        <v>94</v>
+        <v>67</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>94</v>
+        <v>70</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" t="s">
-        <v>94</v>
+        <v>73</v>
+      </c>
+      <c r="C14" s="2">
+        <v>358103070</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>94</v>
+        <v>75</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>94</v>
+        <v>77</v>
+      </c>
+      <c r="C16" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" t="s">
         <v>79</v>
       </c>
-      <c r="B17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>95</v>
+      <c r="C17" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
         <v>81</v>
       </c>
-      <c r="B18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" t="s">
-        <v>94</v>
+      <c r="C18" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -909,30 +936,30 @@
       <c r="B19" t="s">
         <v>84</v>
       </c>
-      <c r="C19" t="s">
-        <v>94</v>
+      <c r="C19" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="C20" s="2">
+        <v>501112222</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -941,10 +968,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3F7E12-4BB4-4905-9EB3-69E34C1A516F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C528FE0E-483D-47BF-B59D-D2610BE7DFFA}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1015,49 +1042,49 @@
         <v>19</v>
       </c>
       <c r="D2" s="1">
-        <v>45663</v>
+        <v>45666</v>
       </c>
       <c r="E2">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="F2">
-        <v>16952</v>
+        <v>81787</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I2">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="K2">
-        <v>4410</v>
+        <v>4940</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="M2">
-        <v>78.95</v>
+        <v>15</v>
       </c>
       <c r="N2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P2">
-        <v>110</v>
+        <v>340</v>
       </c>
       <c r="Q2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="R2">
-        <v>1113</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1071,49 +1098,49 @@
         <v>19</v>
       </c>
       <c r="D3" s="1">
-        <v>45663</v>
+        <v>45666</v>
       </c>
       <c r="E3">
-        <v>270</v>
+        <v>184</v>
       </c>
       <c r="F3">
-        <v>46723</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I3">
         <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K3">
-        <v>4342</v>
+        <v>4340</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="M3">
-        <v>3060</v>
+        <v>26.42</v>
       </c>
       <c r="N3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="P3">
-        <v>310</v>
+        <v>251</v>
       </c>
       <c r="Q3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R3">
-        <v>3100</v>
+        <v>2519</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1127,49 +1154,49 @@
         <v>19</v>
       </c>
       <c r="D4" s="1">
-        <v>45663</v>
+        <v>45666</v>
       </c>
       <c r="E4">
-        <v>799</v>
+        <v>214</v>
       </c>
       <c r="F4">
-        <v>49035</v>
+        <v>25122</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="I4">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
         <v>24</v>
       </c>
       <c r="K4">
-        <v>4600</v>
+        <v>4340</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="M4">
-        <v>1156.54</v>
+        <v>1400</v>
       </c>
       <c r="N4">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="P4">
-        <v>243</v>
+        <v>310</v>
       </c>
       <c r="Q4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="R4">
-        <v>2431</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1183,49 +1210,49 @@
         <v>19</v>
       </c>
       <c r="D5" s="1">
-        <v>45663</v>
+        <v>45666</v>
       </c>
       <c r="E5">
-        <v>988</v>
+        <v>224</v>
       </c>
       <c r="F5">
-        <v>83872</v>
+        <v>46601</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="I5">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="K5">
-        <v>4500</v>
+        <v>1195</v>
       </c>
       <c r="L5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="M5">
+        <v>306.83999999999997</v>
+      </c>
+      <c r="N5">
         <v>80</v>
       </c>
-      <c r="N5">
-        <v>20</v>
-      </c>
       <c r="O5" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="P5">
-        <v>217</v>
+        <v>800</v>
       </c>
       <c r="Q5" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="R5">
-        <v>2180</v>
+        <v>8080</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1239,49 +1266,49 @@
         <v>19</v>
       </c>
       <c r="D6" s="1">
-        <v>45663</v>
+        <v>45666</v>
       </c>
       <c r="E6">
-        <v>1279</v>
+        <v>231</v>
       </c>
       <c r="F6">
-        <v>21582</v>
+        <v>82778</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6">
         <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K6">
-        <v>4410</v>
+        <v>4342</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="M6">
-        <v>1610.85</v>
+        <v>1000</v>
       </c>
       <c r="N6">
         <v>10</v>
       </c>
       <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6">
+        <v>110</v>
+      </c>
+      <c r="Q6" t="s">
         <v>26</v>
       </c>
-      <c r="P6">
-        <v>100</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>54</v>
-      </c>
       <c r="R6">
-        <v>1020</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1295,13 +1322,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="1">
-        <v>45664</v>
+        <v>45666</v>
       </c>
       <c r="E7">
-        <v>161</v>
+        <v>250</v>
       </c>
       <c r="F7">
-        <v>3893</v>
+        <v>9910</v>
       </c>
       <c r="G7" t="s">
         <v>55</v>
@@ -1313,31 +1340,31 @@
         <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K7">
-        <v>4420</v>
+        <v>4390</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="M7">
-        <v>26</v>
+        <v>524.78</v>
       </c>
       <c r="N7">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="O7" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="P7">
-        <v>217</v>
+        <v>380</v>
       </c>
       <c r="Q7" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="R7">
-        <v>2170</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1351,49 +1378,49 @@
         <v>19</v>
       </c>
       <c r="D8" s="1">
-        <v>45664</v>
+        <v>45666</v>
       </c>
       <c r="E8">
-        <v>239</v>
+        <v>263</v>
       </c>
       <c r="F8">
-        <v>65998</v>
+        <v>43245</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="H8" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="I8">
         <v>45</v>
       </c>
       <c r="J8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K8">
-        <v>4600</v>
+        <v>4550</v>
       </c>
       <c r="L8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="M8">
-        <v>34.14</v>
+        <v>33.83</v>
       </c>
       <c r="N8">
         <v>25</v>
       </c>
       <c r="O8" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="P8">
         <v>251</v>
       </c>
       <c r="Q8" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="R8">
-        <v>2511</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1407,49 +1434,49 @@
         <v>19</v>
       </c>
       <c r="D9" s="1">
-        <v>45664</v>
+        <v>45666</v>
       </c>
       <c r="E9">
-        <v>658</v>
+        <v>272</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>33286</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="I9">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J9" t="s">
         <v>20</v>
       </c>
       <c r="K9">
-        <v>4410</v>
+        <v>4510</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="M9">
-        <v>7096.41</v>
+        <v>449.62</v>
       </c>
       <c r="N9">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="O9" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="P9">
-        <v>110</v>
+        <v>241</v>
       </c>
       <c r="Q9" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="R9">
-        <v>1113</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1463,13 +1490,13 @@
         <v>19</v>
       </c>
       <c r="D10" s="1">
-        <v>45665</v>
+        <v>45666</v>
       </c>
       <c r="E10">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="F10">
-        <v>16895</v>
+        <v>89961</v>
       </c>
       <c r="G10" t="s">
         <v>62</v>
@@ -1481,31 +1508,31 @@
         <v>45</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="K10">
-        <v>4601</v>
+        <v>4500</v>
       </c>
       <c r="L10" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="M10">
-        <v>22.93</v>
+        <v>35.68</v>
       </c>
       <c r="N10">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="P10">
-        <v>340</v>
+        <v>217</v>
       </c>
       <c r="Q10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="R10">
-        <v>3427</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1519,49 +1546,49 @@
         <v>19</v>
       </c>
       <c r="D11" s="1">
-        <v>45665</v>
+        <v>45666</v>
       </c>
       <c r="E11">
-        <v>683</v>
+        <v>301</v>
       </c>
       <c r="F11">
-        <v>66408</v>
+        <v>57808</v>
       </c>
       <c r="G11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" t="s">
         <v>65</v>
-      </c>
-      <c r="H11" t="s">
-        <v>66</v>
       </c>
       <c r="I11">
         <v>43</v>
       </c>
       <c r="J11" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K11">
-        <v>4390</v>
+        <v>4342</v>
       </c>
       <c r="L11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="M11">
-        <v>247.15</v>
+        <v>1506</v>
       </c>
       <c r="N11">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="O11" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="P11">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="Q11" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="R11">
-        <v>3602</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1575,49 +1602,49 @@
         <v>19</v>
       </c>
       <c r="D12" s="1">
-        <v>45665</v>
+        <v>45666</v>
       </c>
       <c r="E12">
-        <v>981</v>
+        <v>307</v>
       </c>
       <c r="F12">
-        <v>86898</v>
+        <v>60726</v>
       </c>
       <c r="G12" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12">
+        <v>43</v>
+      </c>
+      <c r="J12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12">
+        <v>4400</v>
+      </c>
+      <c r="L12" t="s">
         <v>68</v>
       </c>
-      <c r="H12" t="s">
-        <v>69</v>
-      </c>
-      <c r="I12">
-        <v>49</v>
-      </c>
-      <c r="J12" t="s">
-        <v>70</v>
-      </c>
-      <c r="K12">
-        <v>4940</v>
-      </c>
-      <c r="L12" t="s">
-        <v>71</v>
-      </c>
       <c r="M12">
-        <v>100</v>
+        <v>899.48</v>
       </c>
       <c r="N12">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="O12" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="P12">
-        <v>243</v>
+        <v>110</v>
       </c>
       <c r="Q12" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="R12">
-        <v>2430</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1634,46 +1661,46 @@
         <v>45666</v>
       </c>
       <c r="E13">
-        <v>165</v>
+        <v>330</v>
       </c>
       <c r="F13">
-        <v>81787</v>
+        <v>26049</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I13">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>24</v>
       </c>
       <c r="K13">
-        <v>4940</v>
+        <v>4470</v>
       </c>
       <c r="L13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M13">
+        <v>139</v>
+      </c>
+      <c r="N13">
+        <v>25</v>
+      </c>
+      <c r="O13" t="s">
+        <v>41</v>
+      </c>
+      <c r="P13">
+        <v>255</v>
+      </c>
+      <c r="Q13" t="s">
         <v>71</v>
       </c>
-      <c r="M13">
-        <v>15</v>
-      </c>
-      <c r="N13">
-        <v>30</v>
-      </c>
-      <c r="O13" t="s">
-        <v>28</v>
-      </c>
-      <c r="P13">
-        <v>340</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>30</v>
-      </c>
       <c r="R13">
-        <v>3431</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1690,46 +1717,46 @@
         <v>45666</v>
       </c>
       <c r="E14">
-        <v>184</v>
+        <v>337</v>
       </c>
       <c r="F14">
-        <v>19</v>
+        <v>37748</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I14">
         <v>43</v>
       </c>
       <c r="J14" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K14">
         <v>4340</v>
       </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="M14">
-        <v>26.42</v>
+        <v>531.25</v>
       </c>
       <c r="N14">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="O14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P14">
-        <v>251</v>
+        <v>380</v>
       </c>
       <c r="Q14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R14">
-        <v>2519</v>
+        <v>3810</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1746,46 +1773,46 @@
         <v>45666</v>
       </c>
       <c r="E15">
-        <v>214</v>
+        <v>349</v>
       </c>
       <c r="F15">
-        <v>25122</v>
+        <v>62839</v>
       </c>
       <c r="G15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I15">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J15" t="s">
         <v>20</v>
       </c>
       <c r="K15">
-        <v>4340</v>
+        <v>4500</v>
       </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="M15">
-        <v>1400</v>
+        <v>266.25</v>
       </c>
       <c r="N15">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="O15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="P15">
-        <v>310</v>
+        <v>217</v>
       </c>
       <c r="Q15" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="R15">
-        <v>3100</v>
+        <v>2182</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1802,46 +1829,46 @@
         <v>45666</v>
       </c>
       <c r="E16">
-        <v>224</v>
+        <v>374</v>
       </c>
       <c r="F16">
-        <v>46601</v>
+        <v>10140</v>
       </c>
       <c r="G16" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="I16">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="J16" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="K16">
-        <v>1195</v>
+        <v>4500</v>
       </c>
       <c r="L16" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="M16">
-        <v>306.83999999999997</v>
+        <v>52.42</v>
       </c>
       <c r="N16">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="O16" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="P16">
-        <v>800</v>
+        <v>217</v>
       </c>
       <c r="Q16" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="R16">
-        <v>8080</v>
+        <v>2181</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1858,46 +1885,46 @@
         <v>45666</v>
       </c>
       <c r="E17">
-        <v>231</v>
+        <v>387</v>
       </c>
       <c r="F17">
-        <v>82778</v>
+        <v>46</v>
       </c>
       <c r="G17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s">
         <v>79</v>
       </c>
-      <c r="H17" t="s">
-        <v>80</v>
-      </c>
       <c r="I17">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s">
         <v>20</v>
       </c>
       <c r="K17">
-        <v>4342</v>
+        <v>4500</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="M17">
-        <v>1000</v>
+        <v>137.06</v>
       </c>
       <c r="N17">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="P17">
-        <v>110</v>
+        <v>217</v>
       </c>
       <c r="Q17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="R17">
-        <v>1106</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1914,46 +1941,46 @@
         <v>45666</v>
       </c>
       <c r="E18">
-        <v>250</v>
+        <v>404</v>
       </c>
       <c r="F18">
-        <v>9910</v>
+        <v>89654</v>
       </c>
       <c r="G18" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" t="s">
         <v>81</v>
       </c>
-      <c r="H18" t="s">
-        <v>82</v>
-      </c>
       <c r="I18">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J18" t="s">
         <v>20</v>
       </c>
       <c r="K18">
-        <v>4390</v>
+        <v>4530</v>
       </c>
       <c r="L18" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
       <c r="M18">
-        <v>524.78</v>
+        <v>258.60000000000002</v>
       </c>
       <c r="N18">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="O18" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="P18">
-        <v>380</v>
+        <v>251</v>
       </c>
       <c r="Q18" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="R18">
-        <v>3810</v>
+        <v>2510</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1970,10 +1997,10 @@
         <v>45666</v>
       </c>
       <c r="E19">
-        <v>263</v>
+        <v>413</v>
       </c>
       <c r="F19">
-        <v>43245</v>
+        <v>1</v>
       </c>
       <c r="G19" t="s">
         <v>83</v>
@@ -1982,34 +2009,34 @@
         <v>84</v>
       </c>
       <c r="I19">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J19" t="s">
         <v>24</v>
       </c>
       <c r="K19">
-        <v>4550</v>
+        <v>4410</v>
       </c>
       <c r="L19" t="s">
         <v>85</v>
       </c>
       <c r="M19">
-        <v>33.83</v>
+        <v>86</v>
       </c>
       <c r="N19">
+        <v>10</v>
+      </c>
+      <c r="O19" t="s">
         <v>25</v>
       </c>
-      <c r="O19" t="s">
-        <v>29</v>
-      </c>
       <c r="P19">
-        <v>251</v>
+        <v>104</v>
       </c>
       <c r="Q19" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="R19">
-        <v>2510</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -2026,46 +2053,46 @@
         <v>45666</v>
       </c>
       <c r="E20">
-        <v>272</v>
+        <v>427</v>
       </c>
       <c r="F20">
-        <v>33286</v>
+        <v>27063</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I20">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J20" t="s">
         <v>24</v>
       </c>
       <c r="K20">
-        <v>4510</v>
+        <v>4470</v>
       </c>
       <c r="L20" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="M20">
-        <v>449.62</v>
+        <v>288.97000000000003</v>
       </c>
       <c r="N20">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="O20" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="P20">
-        <v>241</v>
+        <v>425</v>
       </c>
       <c r="Q20" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="R20">
-        <v>2421</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -2082,46 +2109,46 @@
         <v>45666</v>
       </c>
       <c r="E21">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="F21">
-        <v>89961</v>
+        <v>90811</v>
       </c>
       <c r="G21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I21">
         <v>45</v>
       </c>
       <c r="J21" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21">
+        <v>4600</v>
+      </c>
+      <c r="L21" t="s">
+        <v>93</v>
+      </c>
+      <c r="M21">
+        <v>269.58</v>
+      </c>
+      <c r="N21">
         <v>24</v>
       </c>
-      <c r="K21">
-        <v>4500</v>
-      </c>
-      <c r="L21" t="s">
-        <v>25</v>
-      </c>
-      <c r="M21">
-        <v>35.68</v>
-      </c>
-      <c r="N21">
-        <v>20</v>
-      </c>
       <c r="O21" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="P21">
-        <v>217</v>
+        <v>241</v>
       </c>
       <c r="Q21" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="R21">
-        <v>2174</v>
+        <v>2421</v>
       </c>
     </row>
   </sheetData>
@@ -2130,7 +2157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E07FBD-4DD6-41A6-BF65-804957EF7933}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF76CFFF-39E4-4354-91D8-ED50F2A65150}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>